<commit_message>
updates for sim03... reworking MMU for head pointer to be populated
</commit_message>
<xml_diff>
--- a/sim03/Sim03_355444/Sim03_GradingForm_v01.xlsx
+++ b/sim03/Sim03_355444/Sim03_GradingForm_v01.xlsx
@@ -954,8 +954,8 @@
   </sheetPr>
   <dimension ref="A1:V193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B119" activeCellId="0" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2031,9 +2031,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="119" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1"/>
-      <c r="B119" s="17"/>
+      <c r="B119" s="17" t="n">
+        <v>7</v>
+      </c>
       <c r="C119" s="17"/>
       <c r="D119" s="1" t="s">
         <v>64</v>
@@ -2059,7 +2061,7 @@
       <c r="U119" s="1"/>
       <c r="V119" s="1"/>
     </row>
-    <row r="120" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
       <c r="B120" s="17"/>
       <c r="C120" s="17"/>
@@ -2087,7 +2089,7 @@
       <c r="U120" s="1"/>
       <c r="V120" s="1"/>
     </row>
-    <row r="121" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
       <c r="B121" s="17"/>
       <c r="C121" s="17"/>
@@ -2115,7 +2117,7 @@
       <c r="U121" s="1"/>
       <c r="V121" s="1"/>
     </row>
-    <row r="122" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
       <c r="B122" s="17"/>
       <c r="C122" s="17"/>
@@ -2143,7 +2145,7 @@
       <c r="U122" s="1"/>
       <c r="V122" s="1"/>
     </row>
-    <row r="123" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
       <c r="B123" s="17"/>
       <c r="C123" s="17"/>

</xml_diff>

<commit_message>
working sim03. only issues to fix are with logging to file
</commit_message>
<xml_diff>
--- a/sim03/Sim03_355444/Sim03_GradingForm_v01.xlsx
+++ b/sim03/Sim03_355444/Sim03_GradingForm_v01.xlsx
@@ -954,8 +954,8 @@
   </sheetPr>
   <dimension ref="A1:V193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A100" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B119" activeCellId="0" sqref="B119"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B171" activeCellId="0" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1147,8 +1147,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17"/>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="C26" s="17"/>
       <c r="D26" s="1" t="s">
         <v>21</v>
@@ -1157,8 +1159,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="17"/>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="C27" s="17"/>
       <c r="D27" s="1" t="s">
         <v>21</v>
@@ -1167,8 +1171,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="17"/>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="C28" s="17"/>
       <c r="D28" s="1" t="s">
         <v>21</v>
@@ -1177,8 +1183,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="17"/>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="C29" s="17"/>
       <c r="D29" s="1" t="s">
         <v>21</v>
@@ -1187,8 +1195,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="17"/>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="C30" s="17"/>
       <c r="D30" s="1" t="s">
         <v>21</v>
@@ -1283,8 +1293,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="17"/>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="17" t="n">
+        <v>40</v>
+      </c>
       <c r="C44" s="17"/>
       <c r="D44" s="1" t="s">
         <v>32</v>
@@ -1387,8 +1399,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="17"/>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C59" s="17"/>
       <c r="D59" s="1" t="s">
         <v>39</v>
@@ -1397,8 +1411,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="17"/>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C60" s="17"/>
       <c r="D60" s="1" t="s">
         <v>39</v>
@@ -1407,8 +1423,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="17"/>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C61" s="17"/>
       <c r="D61" s="1" t="s">
         <v>39</v>
@@ -1417,8 +1435,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="17"/>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C62" s="17"/>
       <c r="D62" s="1" t="s">
         <v>39</v>
@@ -1427,8 +1447,10 @@
         <v>43</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="17"/>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B63" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C63" s="17"/>
       <c r="D63" s="1" t="s">
         <v>39</v>
@@ -1502,8 +1524,10 @@
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
     </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="17"/>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B71" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C71" s="17"/>
       <c r="D71" s="1" t="s">
         <v>39</v>
@@ -1512,8 +1536,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="17"/>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C72" s="17"/>
       <c r="D72" s="1" t="s">
         <v>46</v>
@@ -1522,8 +1548,10 @@
         <v>47</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="17"/>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="C73" s="17"/>
       <c r="D73" s="1" t="s">
         <v>39</v>
@@ -1597,8 +1625,10 @@
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="17"/>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B81" s="17" t="n">
+        <v>10</v>
+      </c>
       <c r="C81" s="17"/>
       <c r="D81" s="1" t="s">
         <v>49</v>
@@ -1607,8 +1637,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="17"/>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="17" t="n">
+        <v>10</v>
+      </c>
       <c r="C82" s="17"/>
       <c r="D82" s="1" t="s">
         <v>49</v>
@@ -1617,8 +1649,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="17"/>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B83" s="17" t="n">
+        <v>10</v>
+      </c>
       <c r="C83" s="17"/>
       <c r="D83" s="1" t="s">
         <v>49</v>
@@ -1710,9 +1744,11 @@
         <v>54</v>
       </c>
     </row>
-    <row r="94" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1"/>
-      <c r="B94" s="17"/>
+      <c r="B94" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C94" s="17"/>
       <c r="D94" s="1" t="s">
         <v>39</v>
@@ -1738,9 +1774,11 @@
       <c r="U94" s="1"/>
       <c r="V94" s="1"/>
     </row>
-    <row r="95" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="1"/>
-      <c r="B95" s="17"/>
+      <c r="B95" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C95" s="17"/>
       <c r="D95" s="1" t="s">
         <v>39</v>
@@ -1837,9 +1875,11 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1"/>
-      <c r="B105" s="17"/>
+      <c r="B105" s="17" t="n">
+        <v>10</v>
+      </c>
       <c r="C105" s="17"/>
       <c r="D105" s="1" t="s">
         <v>49</v>
@@ -1865,9 +1905,11 @@
       <c r="U105" s="1"/>
       <c r="V105" s="1"/>
     </row>
-    <row r="106" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1"/>
-      <c r="B106" s="17"/>
+      <c r="B106" s="17" t="n">
+        <v>10</v>
+      </c>
       <c r="C106" s="17"/>
       <c r="D106" s="1" t="s">
         <v>49</v>
@@ -1893,9 +1935,11 @@
       <c r="U106" s="1"/>
       <c r="V106" s="1"/>
     </row>
-    <row r="107" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="1"/>
-      <c r="B107" s="17"/>
+      <c r="B107" s="17" t="n">
+        <v>10</v>
+      </c>
       <c r="C107" s="17"/>
       <c r="D107" s="1" t="s">
         <v>49</v>
@@ -1921,9 +1965,11 @@
       <c r="U107" s="1"/>
       <c r="V107" s="1"/>
     </row>
-    <row r="108" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="1"/>
-      <c r="B108" s="17"/>
+      <c r="B108" s="17" t="n">
+        <v>10</v>
+      </c>
       <c r="C108" s="17"/>
       <c r="D108" s="1" t="s">
         <v>49</v>
@@ -2063,7 +2109,9 @@
     </row>
     <row r="120" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1"/>
-      <c r="B120" s="17"/>
+      <c r="B120" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C120" s="17"/>
       <c r="D120" s="1" t="s">
         <v>39</v>
@@ -2091,7 +2139,9 @@
     </row>
     <row r="121" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1"/>
-      <c r="B121" s="17"/>
+      <c r="B121" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C121" s="17"/>
       <c r="D121" s="1" t="s">
         <v>39</v>
@@ -2119,7 +2169,9 @@
     </row>
     <row r="122" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="1"/>
-      <c r="B122" s="17"/>
+      <c r="B122" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C122" s="17"/>
       <c r="D122" s="1" t="s">
         <v>39</v>
@@ -2147,7 +2199,9 @@
     </row>
     <row r="123" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="1"/>
-      <c r="B123" s="17"/>
+      <c r="B123" s="17" t="n">
+        <v>5</v>
+      </c>
       <c r="C123" s="17"/>
       <c r="D123" s="1" t="s">
         <v>39</v>
@@ -2254,7 +2308,9 @@
     </row>
     <row r="134" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1"/>
-      <c r="B134" s="17"/>
+      <c r="B134" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C134" s="17"/>
       <c r="D134" s="1" t="s">
         <v>73</v>
@@ -2282,7 +2338,9 @@
     </row>
     <row r="135" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1"/>
-      <c r="B135" s="17"/>
+      <c r="B135" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C135" s="17"/>
       <c r="D135" s="1" t="s">
         <v>73</v>
@@ -2310,7 +2368,9 @@
     </row>
     <row r="136" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1"/>
-      <c r="B136" s="17"/>
+      <c r="B136" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C136" s="17"/>
       <c r="D136" s="1" t="s">
         <v>73</v>
@@ -2338,7 +2398,9 @@
     </row>
     <row r="137" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1"/>
-      <c r="B137" s="17"/>
+      <c r="B137" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C137" s="17"/>
       <c r="D137" s="1" t="s">
         <v>77</v>
@@ -2366,7 +2428,9 @@
     </row>
     <row r="138" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1"/>
-      <c r="B138" s="17"/>
+      <c r="B138" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C138" s="17"/>
       <c r="D138" s="1" t="s">
         <v>77</v>
@@ -2394,7 +2458,9 @@
     </row>
     <row r="139" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1"/>
-      <c r="B139" s="17"/>
+      <c r="B139" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C139" s="17"/>
       <c r="D139" s="1" t="s">
         <v>77</v>
@@ -2422,7 +2488,9 @@
     </row>
     <row r="140" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="1"/>
-      <c r="B140" s="17"/>
+      <c r="B140" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C140" s="17"/>
       <c r="D140" s="1" t="s">
         <v>77</v>
@@ -2450,7 +2518,9 @@
     </row>
     <row r="141" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="1"/>
-      <c r="B141" s="17"/>
+      <c r="B141" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C141" s="17"/>
       <c r="D141" s="1" t="s">
         <v>77</v>
@@ -2478,7 +2548,9 @@
     </row>
     <row r="142" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="1"/>
-      <c r="B142" s="17"/>
+      <c r="B142" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C142" s="17"/>
       <c r="D142" s="1" t="s">
         <v>77</v>
@@ -2506,7 +2578,9 @@
     </row>
     <row r="143" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="1"/>
-      <c r="B143" s="17"/>
+      <c r="B143" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C143" s="17"/>
       <c r="D143" s="1" t="s">
         <v>77</v>
@@ -2534,7 +2608,9 @@
     </row>
     <row r="144" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="1"/>
-      <c r="B144" s="17"/>
+      <c r="B144" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C144" s="17"/>
       <c r="D144" s="1" t="s">
         <v>77</v>
@@ -2562,7 +2638,9 @@
     </row>
     <row r="145" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="1"/>
-      <c r="B145" s="17"/>
+      <c r="B145" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C145" s="17"/>
       <c r="D145" s="1" t="s">
         <v>86</v>
@@ -2590,7 +2668,9 @@
     </row>
     <row r="146" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="1"/>
-      <c r="B146" s="17"/>
+      <c r="B146" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C146" s="17"/>
       <c r="D146" s="1" t="s">
         <v>86</v>
@@ -2618,7 +2698,9 @@
     </row>
     <row r="147" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="1"/>
-      <c r="B147" s="17"/>
+      <c r="B147" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C147" s="17"/>
       <c r="D147" s="1" t="s">
         <v>86</v>
@@ -2646,7 +2728,9 @@
     </row>
     <row r="148" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="1"/>
-      <c r="B148" s="17"/>
+      <c r="B148" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C148" s="17"/>
       <c r="D148" s="1" t="s">
         <v>86</v>
@@ -2674,7 +2758,9 @@
     </row>
     <row r="149" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="1"/>
-      <c r="B149" s="17"/>
+      <c r="B149" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C149" s="17"/>
       <c r="D149" s="1" t="s">
         <v>86</v>
@@ -2702,7 +2788,9 @@
     </row>
     <row r="150" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1"/>
-      <c r="B150" s="17"/>
+      <c r="B150" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C150" s="17"/>
       <c r="D150" s="1" t="s">
         <v>86</v>
@@ -2730,7 +2818,9 @@
     </row>
     <row r="151" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="1"/>
-      <c r="B151" s="17"/>
+      <c r="B151" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C151" s="17"/>
       <c r="D151" s="1" t="s">
         <v>86</v>
@@ -2786,7 +2876,9 @@
       <c r="D156" s="16"/>
     </row>
     <row r="157" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B157" s="17"/>
+      <c r="B157" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C157" s="17"/>
       <c r="D157" s="16"/>
       <c r="E157" s="1" t="s">
@@ -2917,7 +3009,9 @@
     </row>
     <row r="167" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="1"/>
-      <c r="B167" s="17"/>
+      <c r="B167" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C167" s="17" t="n">
         <v>0</v>
       </c>
@@ -2947,7 +3041,9 @@
     </row>
     <row r="168" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="1"/>
-      <c r="B168" s="17"/>
+      <c r="B168" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C168" s="17" t="n">
         <v>0</v>
       </c>
@@ -2977,7 +3073,9 @@
     </row>
     <row r="169" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="1"/>
-      <c r="B169" s="17"/>
+      <c r="B169" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C169" s="17" t="n">
         <v>0</v>
       </c>
@@ -3007,7 +3105,9 @@
     </row>
     <row r="170" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="1"/>
-      <c r="B170" s="17"/>
+      <c r="B170" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C170" s="17" t="n">
         <v>0</v>
       </c>
@@ -3037,7 +3137,9 @@
     </row>
     <row r="171" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="1"/>
-      <c r="B171" s="17"/>
+      <c r="B171" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C171" s="17" t="n">
         <v>0</v>
       </c>
@@ -3067,7 +3169,9 @@
     </row>
     <row r="172" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="1"/>
-      <c r="B172" s="17"/>
+      <c r="B172" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C172" s="17" t="n">
         <v>0</v>
       </c>
@@ -3097,7 +3201,9 @@
     </row>
     <row r="173" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="1"/>
-      <c r="B173" s="17"/>
+      <c r="B173" s="17" t="n">
+        <v>0</v>
+      </c>
       <c r="C173" s="17" t="n">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
working final version of sim03....
</commit_message>
<xml_diff>
--- a/sim03/Sim03_355444/Sim03_GradingForm_v01.xlsx
+++ b/sim03/Sim03_355444/Sim03_GradingForm_v01.xlsx
@@ -954,8 +954,8 @@
   </sheetPr>
   <dimension ref="A1:V193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B171" activeCellId="0" sqref="B171"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K90" activeCellId="0" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1550,7 +1550,7 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B73" s="17" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C73" s="17"/>
       <c r="D73" s="1" t="s">
@@ -2080,7 +2080,7 @@
     <row r="119" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="1"/>
       <c r="B119" s="17" t="n">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C119" s="17"/>
       <c r="D119" s="1" t="s">

</xml_diff>